<commit_message>
2024 08 13 추가 수정
</commit_message>
<xml_diff>
--- a/fitness/src/main/webapp/dbfile/db설계.xlsx
+++ b/fitness/src/main/webapp/dbfile/db설계.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tj-bu-708-00\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaya8\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1899DCA6-FC5F-4C16-9453-4CC9DCF5D6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29878A74-CC68-4F9A-BF48-62D062CF54B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="27465" windowHeight="13710" xr2:uid="{3716DFE8-E011-4722-8171-A90C407EC680}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3716DFE8-E011-4722-8171-A90C407EC680}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="100">
   <si>
     <t>컬럼명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -337,10 +337,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DESCRIPTION</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로그램 번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -349,10 +345,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>프로그램 설명</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>INSTRUCTOR_ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -417,6 +409,18 @@
   </si>
   <si>
     <t>CONTENTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로그램번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROGRAM_ENAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프로그램 영문명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -833,7 +837,7 @@
   <dimension ref="A2:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -849,7 +853,7 @@
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -994,7 +998,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
@@ -1003,7 +1007,7 @@
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
         <v>30</v>
@@ -1094,7 +1098,7 @@
         <v>56</v>
       </c>
       <c r="I8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
@@ -1152,33 +1156,33 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
         <v>92</v>
       </c>
-      <c r="B11" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" t="s">
-        <v>94</v>
-      </c>
       <c r="E11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1192,7 +1196,7 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
@@ -1201,7 +1205,7 @@
         <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1215,10 +1219,10 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1245,13 +1249,13 @@
     </row>
     <row r="16" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1318,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N18" t="s">
         <v>23</v>
@@ -1327,7 +1331,7 @@
         <v>26</v>
       </c>
       <c r="P18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -1371,10 +1375,10 @@
         <v>77</v>
       </c>
       <c r="N19" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="P19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -1412,27 +1416,27 @@
         <v>46</v>
       </c>
       <c r="M20" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="N20" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="P20" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
@@ -1458,16 +1462,16 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E22" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
2024 08 14 DB 추가
</commit_message>
<xml_diff>
--- a/fitness/src/main/webapp/dbfile/db설계.xlsx
+++ b/fitness/src/main/webapp/dbfile/db설계.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaya8\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tj-bu-708-00\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29878A74-CC68-4F9A-BF48-62D062CF54B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF657FCA-D169-49AA-B90F-A2A54A116833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3716DFE8-E011-4722-8171-A90C407EC680}"/>
+    <workbookView xWindow="510" yWindow="285" windowWidth="27465" windowHeight="13725" xr2:uid="{3716DFE8-E011-4722-8171-A90C407EC680}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="107">
   <si>
     <t>컬럼명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -245,14 +245,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CLASS_NAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강의제목</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VARCHAR(30)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -396,10 +388,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RROGRAMNO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PROGRAMNO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -421,6 +409,46 @@
   </si>
   <si>
     <t>프로그램 영문명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>강의번호(BOARDNO와 연결)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CDATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UDATETIME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작성일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수정일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLASS_NUM_CNT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수강신청인원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ENROLLNO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수강신청번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHAR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,12 +473,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -504,7 +538,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -519,6 +553,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A143954-A68B-4E5F-BE5E-D12E9386031A}">
   <dimension ref="A2:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -860,29 +906,29 @@
     <row r="2" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="4"/>
       <c r="I3" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="4"/>
+      <c r="M3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="7"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -924,16 +970,16 @@
       <c r="L4" t="s">
         <v>3</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -960,7 +1006,7 @@
         <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>
@@ -974,16 +1020,16 @@
       <c r="L5" t="s">
         <v>52</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="8" t="s">
         <v>51</v>
       </c>
     </row>
@@ -998,7 +1044,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
@@ -1007,7 +1053,7 @@
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
         <v>30</v>
@@ -1021,16 +1067,16 @@
       <c r="L6" t="s">
         <v>12</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="P6" t="s">
+      <c r="P6" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1065,16 +1111,16 @@
       <c r="L7" t="s">
         <v>33</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1089,16 +1135,16 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
@@ -1106,13 +1152,14 @@
       <c r="L8" t="s">
         <v>34</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="P8" t="s">
+      <c r="O8" s="8"/>
+      <c r="P8" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1127,13 +1174,13 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>48</v>
+        <v>103</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1156,33 +1203,51 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" t="s">
         <v>85</v>
+      </c>
+      <c r="L10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
         <v>90</v>
       </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" t="s">
-        <v>92</v>
-      </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="I11" t="s">
+        <v>99</v>
+      </c>
+      <c r="J11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1196,16 +1261,16 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
         <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1219,10 +1284,13 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="F13" t="s">
+        <v>106</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1230,7 +1298,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -1238,47 +1306,47 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
       <c r="I17" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="4"/>
       <c r="M17" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1322,30 +1390,30 @@
         <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="P18" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
         <v>39</v>
@@ -1372,27 +1440,30 @@
         <v>44</v>
       </c>
       <c r="M19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="N19" t="s">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="O19" t="s">
+        <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -1416,27 +1487,27 @@
         <v>46</v>
       </c>
       <c r="M20" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="N20" t="s">
         <v>21</v>
       </c>
       <c r="P20" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
         <v>30</v>
@@ -1451,56 +1522,53 @@
         <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J21" t="s">
         <v>21</v>
       </c>
       <c r="L21" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="M21" t="s">
+        <v>95</v>
+      </c>
+      <c r="N21" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
       <c r="H23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024 08 20 작업
</commit_message>
<xml_diff>
--- a/fitness/src/main/webapp/dbfile/db설계.xlsx
+++ b/fitness/src/main/webapp/dbfile/db설계.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tj-bu-708-00\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF657FCA-D169-49AA-B90F-A2A54A116833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0955DE4C-0537-45E2-A2B8-99CAE390CCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="510" yWindow="285" windowWidth="27465" windowHeight="13725" xr2:uid="{3716DFE8-E011-4722-8171-A90C407EC680}"/>
   </bookViews>
@@ -261,18 +261,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TBL_COMMENT(댓글정보)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TBL_ENROLL(수강신청정보)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TBL_CLASS_LIST(수강내역)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TBL_ROOM(강의실정보)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -449,6 +441,14 @@
   </si>
   <si>
     <t>CHAR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBL_CLASS_LIST(수강내역) - 불필요 폐기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBL_COMMENT(댓글정보) - 추후 작업</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -473,7 +473,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,7 +482,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.249977111117893"/>
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,7 +544,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -564,6 +570,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -883,7 +901,7 @@
   <dimension ref="A2:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -923,12 +941,12 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
-      <c r="M3" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="7"/>
+      <c r="M3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="11"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
@@ -970,16 +988,16 @@
       <c r="L4" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1006,7 +1024,7 @@
         <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I5" t="s">
         <v>27</v>
@@ -1020,16 +1038,16 @@
       <c r="L5" t="s">
         <v>52</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="12" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1044,7 +1062,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" t="s">
         <v>23</v>
@@ -1053,7 +1071,7 @@
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I6" t="s">
         <v>30</v>
@@ -1067,16 +1085,16 @@
       <c r="L6" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="12" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1111,16 +1129,16 @@
       <c r="L7" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="12" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1144,7 +1162,7 @@
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J8" t="s">
         <v>50</v>
@@ -1152,14 +1170,14 @@
       <c r="L8" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="8" t="s">
+      <c r="N8" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8" t="s">
+      <c r="O8" s="12"/>
+      <c r="P8" s="12" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1174,13 +1192,13 @@
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I9" t="s">
         <v>32</v>
@@ -1203,51 +1221,51 @@
         <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" t="s">
         <v>83</v>
       </c>
-      <c r="I10" t="s">
+      <c r="L10" t="s">
         <v>98</v>
-      </c>
-      <c r="J10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" t="s">
         <v>88</v>
       </c>
-      <c r="B11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" t="s">
-        <v>90</v>
-      </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" t="s">
+        <v>83</v>
+      </c>
+      <c r="L11" t="s">
         <v>99</v>
-      </c>
-      <c r="J11" t="s">
-        <v>85</v>
-      </c>
-      <c r="L11" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1261,7 +1279,7 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" t="s">
         <v>55</v>
@@ -1270,7 +1288,7 @@
         <v>29</v>
       </c>
       <c r="H12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1284,13 +1302,13 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1298,7 +1316,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
@@ -1306,47 +1324,47 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="4"/>
+      <c r="E17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
       <c r="I17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="4"/>
       <c r="M17" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
@@ -1365,16 +1383,16 @@
       <c r="D18" t="s">
         <v>3</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="8" t="s">
         <v>3</v>
       </c>
       <c r="I18" t="s">
@@ -1404,7 +1422,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
         <v>23</v>
@@ -1413,18 +1431,18 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="8" t="s">
         <v>41</v>
       </c>
       <c r="I19" t="s">
@@ -1440,7 +1458,7 @@
         <v>44</v>
       </c>
       <c r="M19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N19" t="s">
         <v>23</v>
@@ -1449,7 +1467,7 @@
         <v>26</v>
       </c>
       <c r="P19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -1465,16 +1483,16 @@
       <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="8" t="s">
         <v>42</v>
       </c>
       <c r="I20" t="s">
@@ -1487,13 +1505,13 @@
         <v>46</v>
       </c>
       <c r="M20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="N20" t="s">
         <v>21</v>
       </c>
       <c r="P20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
@@ -1509,66 +1527,68 @@
       <c r="D21" t="s">
         <v>42</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="8" t="s">
         <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J21" t="s">
         <v>21</v>
       </c>
       <c r="L21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="N21" t="s">
         <v>21</v>
       </c>
       <c r="P21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F22" t="s">
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="E23" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
+      <c r="G23" s="8"/>
+      <c r="H23" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="F23" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>